<commit_message>
Manual y casos de prueba listos
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -102,9 +102,6 @@
     <t xml:space="preserve">El sistema hace los jobs correctamente </t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema tiene una bitácora con los cambios de claves de usuarios </t>
-  </si>
-  <si>
     <t>El sistema permite ver los datos de su propia cuenta</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Las busquedas estan ordenadas alfabeticamente</t>
   </si>
   <si>
-    <t>Los mensajes de correo deben ser parametrizables</t>
-  </si>
-  <si>
     <t>La clave debe estar guardarse encriptada</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t xml:space="preserve">El sistema debe registrar la información completa </t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Permite ver la galería de fotos de todos los usuarios</t>
   </si>
 </sst>
 </file>
@@ -242,8 +242,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -313,6 +319,9 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -334,6 +343,9 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -704,8 +716,11 @@
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -716,10 +731,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -730,10 +745,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -744,10 +759,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -758,10 +773,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -772,10 +787,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -786,10 +801,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -800,10 +815,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -814,10 +829,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -828,10 +843,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -842,10 +857,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -856,10 +871,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -870,10 +885,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -884,10 +899,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -898,10 +913,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -912,10 +927,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -926,10 +941,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -940,10 +955,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -954,10 +969,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -968,24 +983,24 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -996,7 +1011,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
@@ -1004,11 +1019,13 @@
       <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
@@ -1022,7 +1039,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -1036,7 +1053,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
@@ -1050,7 +1067,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
@@ -1064,9 +1081,9 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C29" t="s">
@@ -1078,7 +1095,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -1092,7 +1109,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>34</v>
@@ -1106,7 +1123,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>35</v>
@@ -1120,7 +1137,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>36</v>
@@ -1134,7 +1151,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
@@ -1148,7 +1165,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>38</v>
@@ -1156,13 +1173,13 @@
       <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>39</v>
@@ -1176,7 +1193,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>40</v>
@@ -1190,7 +1207,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>41</v>
@@ -1204,21 +1221,21 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
@@ -1232,10 +1249,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1246,10 +1263,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1260,10 +1277,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1274,109 +1291,115 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>